<commit_message>
I think I have broken it down and understand
</commit_message>
<xml_diff>
--- a/CH-167 Table Transformation.xlsx
+++ b/CH-167 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D72745A-3CC0-40BC-9499-7BA9B4820C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDF2754-75DE-4D51-BBFA-86AAD1E63F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -484,6 +484,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,7 +635,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>143363</xdr:colOff>
+      <xdr:colOff>44303</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>93607</xdr:rowOff>
     </xdr:to>
@@ -1530,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF92CE75-0CD4-452E-A14B-B406E02DE003}">
-  <dimension ref="B1:N27"/>
+  <dimension ref="B1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1542,6 +1543,7 @@
     <col min="3" max="3" width="12.3984375" style="5" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="9" customWidth="1"/>
     <col min="5" max="7" width="10.5" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1865,7 +1867,7 @@
         <v>=0&gt;""</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" s="27" t="s">
         <v>2</v>
       </c>
@@ -1885,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" s="27" t="s">
         <v>3</v>
       </c>
@@ -1905,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" s="27" t="s">
         <v>4</v>
       </c>
@@ -1924,8 +1926,28 @@
       <c r="J19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="b" cm="1">
+        <f t="array" ref="K19:K43">C3:C27&gt;""</f>
+        <v>0</v>
+      </c>
+      <c r="L19" cm="1">
+        <f t="array" ref="L19:L43">_xlfn.SCAN(,C3:C27,_xleta.MAX)</f>
+        <v>45493</v>
+      </c>
+      <c r="M19" cm="1">
+        <f t="array" ref="M19:M28">_xlfn._xlws.FILTER(_xlfn.SCAN(,C3:C27,_xleta.MAX),C3:C27&gt;"")</f>
+        <v>45493</v>
+      </c>
+      <c r="O19" s="36" cm="1">
+        <f t="array" ref="O19:O23">C3:C7</f>
+        <v>45493</v>
+      </c>
+      <c r="Q19" t="str" cm="1">
+        <f t="array" ref="Q19:Q28">_xlfn._xlws.FILTER(C3:C27,C3:C27&gt;"")</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="28">
         <v>5</v>
       </c>
@@ -1944,8 +1966,23 @@
       <c r="J20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>45493</v>
+      </c>
+      <c r="M20">
+        <v>45509</v>
+      </c>
+      <c r="O20" s="36" t="str">
+        <v>A</v>
+      </c>
+      <c r="Q20" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" s="28">
         <v>4</v>
       </c>
@@ -1964,8 +2001,23 @@
       <c r="J21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>45493</v>
+      </c>
+      <c r="M21">
+        <v>45509</v>
+      </c>
+      <c r="O21" s="36">
+        <v>10</v>
+      </c>
+      <c r="Q21" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="28">
         <v>3</v>
       </c>
@@ -1984,8 +2036,23 @@
       <c r="J22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>45509</v>
+      </c>
+      <c r="M22">
+        <v>45509</v>
+      </c>
+      <c r="O22">
+        <v>45509</v>
+      </c>
+      <c r="Q22" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" s="25">
         <v>45566</v>
       </c>
@@ -2004,8 +2071,23 @@
       <c r="J23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>45509</v>
+      </c>
+      <c r="M23">
+        <v>45517</v>
+      </c>
+      <c r="O23" t="str">
+        <v>C</v>
+      </c>
+      <c r="Q23" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" s="25" t="s">
         <v>2</v>
       </c>
@@ -2024,8 +2106,20 @@
       <c r="J24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>45509</v>
+      </c>
+      <c r="M24">
+        <v>45553</v>
+      </c>
+      <c r="Q24" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C25" s="25" t="s">
         <v>3</v>
       </c>
@@ -2044,8 +2138,20 @@
       <c r="J25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>45509</v>
+      </c>
+      <c r="M25">
+        <v>45553</v>
+      </c>
+      <c r="Q25" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C26" s="26">
         <v>1</v>
       </c>
@@ -2055,8 +2161,20 @@
       <c r="J26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>45509</v>
+      </c>
+      <c r="M26">
+        <v>45553</v>
+      </c>
+      <c r="Q26" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" s="29">
         <v>2</v>
       </c>
@@ -2065,6 +2183,152 @@
       </c>
       <c r="J27" t="b">
         <v>0</v>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>45509</v>
+      </c>
+      <c r="M27">
+        <v>45566</v>
+      </c>
+      <c r="Q27" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>45509</v>
+      </c>
+      <c r="M28">
+        <v>45566</v>
+      </c>
+      <c r="Q28" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K29" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K31" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="34" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="35" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="36" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K36" t="b">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="37" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K37" t="b">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="38" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K38" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="39" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="40" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="41" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="42" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K42" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="43" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>45566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>